<commit_message>
Update decimals performance analysis;
</commit_message>
<xml_diff>
--- a/decimals.xlsx
+++ b/decimals.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="scale=2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="scale=4" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="scale=6" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Sheet4" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">results!$A$1:$C$40</definedName>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>precision</t>
   </si>
@@ -25,6 +26,12 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>base-10 digits</t>
   </si>
 </sst>
 </file>
@@ -58,13 +65,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -111,11 +119,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="395233934"/>
-        <c:axId val="1905940396"/>
+        <c:axId val="1674854533"/>
+        <c:axId val="1822926803"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="395233934"/>
+        <c:axId val="1674854533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -167,10 +175,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1905940396"/>
+        <c:crossAx val="1822926803"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1905940396"/>
+        <c:axId val="1822926803"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -245,7 +253,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="395233934"/>
+        <c:crossAx val="1674854533"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -309,11 +317,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="379936453"/>
-        <c:axId val="194301494"/>
+        <c:axId val="1658399600"/>
+        <c:axId val="177899596"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="379936453"/>
+        <c:axId val="1658399600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -365,10 +373,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194301494"/>
+        <c:crossAx val="177899596"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194301494"/>
+        <c:axId val="177899596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -443,7 +451,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="379936453"/>
+        <c:crossAx val="1658399600"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -507,11 +515,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="753861382"/>
-        <c:axId val="614287134"/>
+        <c:axId val="714521236"/>
+        <c:axId val="1350105701"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="753861382"/>
+        <c:axId val="714521236"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,10 +571,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="614287134"/>
+        <c:crossAx val="1350105701"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="614287134"/>
+        <c:axId val="1350105701"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -641,7 +649,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="753861382"/>
+        <c:crossAx val="714521236"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -759,6 +767,10 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -976,7 +988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="1">
       <c r="A2" s="1">
         <v>8.0</v>
       </c>
@@ -984,10 +996,10 @@
         <v>2.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1.603</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1.834</v>
+      </c>
+    </row>
+    <row r="3" hidden="1">
       <c r="A3" s="1">
         <v>9.0</v>
       </c>
@@ -995,10 +1007,10 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1">
-        <v>1.645</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1.531</v>
+      </c>
+    </row>
+    <row r="4" hidden="1">
       <c r="A4" s="1">
         <v>9.0</v>
       </c>
@@ -1006,10 +1018,10 @@
         <v>4.0</v>
       </c>
       <c r="C4" s="1">
-        <v>1.756</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>1.746</v>
+      </c>
+    </row>
+    <row r="5" hidden="1">
       <c r="A5" s="1">
         <v>10.0</v>
       </c>
@@ -1017,10 +1029,10 @@
         <v>2.0</v>
       </c>
       <c r="C5" s="1">
-        <v>1.839</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="6" hidden="1">
       <c r="A6" s="1">
         <v>10.0</v>
       </c>
@@ -1028,10 +1040,10 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="1">
-        <v>3.324</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1.661</v>
+      </c>
+    </row>
+    <row r="7" hidden="1">
       <c r="A7" s="1">
         <v>11.0</v>
       </c>
@@ -1039,10 +1051,10 @@
         <v>2.0</v>
       </c>
       <c r="C7" s="1">
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>1.533</v>
+      </c>
+    </row>
+    <row r="8" hidden="1">
       <c r="A8" s="1">
         <v>11.0</v>
       </c>
@@ -1050,10 +1062,10 @@
         <v>4.0</v>
       </c>
       <c r="C8" s="1">
-        <v>3.283</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1.696</v>
+      </c>
+    </row>
+    <row r="9" hidden="1">
       <c r="A9" s="1">
         <v>12.0</v>
       </c>
@@ -1061,10 +1073,10 @@
         <v>2.0</v>
       </c>
       <c r="C9" s="1">
-        <v>1.874</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1.539</v>
+      </c>
+    </row>
+    <row r="10" hidden="1">
       <c r="A10" s="1">
         <v>12.0</v>
       </c>
@@ -1072,10 +1084,10 @@
         <v>4.0</v>
       </c>
       <c r="C10" s="1">
-        <v>3.374</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>1.993</v>
+      </c>
+    </row>
+    <row r="11" hidden="1">
       <c r="A11" s="1">
         <v>13.0</v>
       </c>
@@ -1083,10 +1095,10 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="1">
-        <v>1.895</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="12" hidden="1">
       <c r="A12" s="1">
         <v>13.0</v>
       </c>
@@ -1094,10 +1106,10 @@
         <v>4.0</v>
       </c>
       <c r="C12" s="1">
-        <v>3.392</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>1.893</v>
+      </c>
+    </row>
+    <row r="13" hidden="1">
       <c r="A13" s="1">
         <v>14.0</v>
       </c>
@@ -1105,10 +1117,10 @@
         <v>2.0</v>
       </c>
       <c r="C13" s="1">
-        <v>1.906</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>1.654</v>
+      </c>
+    </row>
+    <row r="14" hidden="1">
       <c r="A14" s="1">
         <v>14.0</v>
       </c>
@@ -1116,10 +1128,10 @@
         <v>4.0</v>
       </c>
       <c r="C14" s="1">
-        <v>3.406</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1.628</v>
+      </c>
+    </row>
+    <row r="15" hidden="1">
       <c r="A15" s="1">
         <v>15.0</v>
       </c>
@@ -1127,10 +1139,10 @@
         <v>2.0</v>
       </c>
       <c r="C15" s="1">
-        <v>1.853</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>1.552</v>
+      </c>
+    </row>
+    <row r="16" hidden="1">
       <c r="A16" s="1">
         <v>15.0</v>
       </c>
@@ -1138,10 +1150,10 @@
         <v>4.0</v>
       </c>
       <c r="C16" s="1">
-        <v>3.385</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>2.025</v>
+      </c>
+    </row>
+    <row r="17" hidden="1">
       <c r="A17" s="1">
         <v>16.0</v>
       </c>
@@ -1149,10 +1161,10 @@
         <v>2.0</v>
       </c>
       <c r="C17" s="1">
-        <v>1.869</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1.582</v>
+      </c>
+    </row>
+    <row r="18" hidden="1">
       <c r="A18" s="1">
         <v>16.0</v>
       </c>
@@ -1160,7 +1172,7 @@
         <v>4.0</v>
       </c>
       <c r="C18" s="1">
-        <v>3.386</v>
+        <v>1.901</v>
       </c>
     </row>
     <row r="19">
@@ -1171,10 +1183,10 @@
         <v>6.0</v>
       </c>
       <c r="C19" s="1">
-        <v>2.163</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>2.028</v>
+      </c>
+    </row>
+    <row r="20" hidden="1">
       <c r="A20" s="1">
         <v>17.0</v>
       </c>
@@ -1182,10 +1194,10 @@
         <v>2.0</v>
       </c>
       <c r="C20" s="1">
-        <v>1.864</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1.507</v>
+      </c>
+    </row>
+    <row r="21" hidden="1">
       <c r="A21" s="1">
         <v>17.0</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>4.0</v>
       </c>
       <c r="C21" s="1">
-        <v>3.409</v>
+        <v>1.771</v>
       </c>
     </row>
     <row r="22">
@@ -1204,10 +1216,10 @@
         <v>6.0</v>
       </c>
       <c r="C22" s="1">
-        <v>2.119</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>2.115</v>
+      </c>
+    </row>
+    <row r="23" hidden="1">
       <c r="A23" s="1">
         <v>18.0</v>
       </c>
@@ -1215,10 +1227,10 @@
         <v>2.0</v>
       </c>
       <c r="C23" s="1">
-        <v>1.895</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1.521</v>
+      </c>
+    </row>
+    <row r="24" hidden="1">
       <c r="A24" s="1">
         <v>18.0</v>
       </c>
@@ -1226,7 +1238,7 @@
         <v>4.0</v>
       </c>
       <c r="C24" s="1">
-        <v>3.424</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="25">
@@ -1237,10 +1249,10 @@
         <v>6.0</v>
       </c>
       <c r="C25" s="1">
-        <v>2.195</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>2.287</v>
+      </c>
+    </row>
+    <row r="26" hidden="1">
       <c r="A26" s="1">
         <v>19.0</v>
       </c>
@@ -1248,10 +1260,10 @@
         <v>2.0</v>
       </c>
       <c r="C26" s="1">
-        <v>3.74</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="27" hidden="1">
       <c r="A27" s="1">
         <v>19.0</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>4.0</v>
       </c>
       <c r="C27" s="1">
-        <v>3.665</v>
+        <v>2.734</v>
       </c>
     </row>
     <row r="28">
@@ -1270,10 +1282,10 @@
         <v>6.0</v>
       </c>
       <c r="C28" s="1">
-        <v>3.023</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>3.044</v>
+      </c>
+    </row>
+    <row r="29" hidden="1">
       <c r="A29" s="1">
         <v>20.0</v>
       </c>
@@ -1281,10 +1293,10 @@
         <v>2.0</v>
       </c>
       <c r="C29" s="1">
-        <v>3.647</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>2.968</v>
+      </c>
+    </row>
+    <row r="30" hidden="1">
       <c r="A30" s="1">
         <v>20.0</v>
       </c>
@@ -1292,7 +1304,7 @@
         <v>4.0</v>
       </c>
       <c r="C30" s="1">
-        <v>3.606</v>
+        <v>2.773</v>
       </c>
     </row>
     <row r="31">
@@ -1303,10 +1315,10 @@
         <v>6.0</v>
       </c>
       <c r="C31" s="1">
-        <v>3.068</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>3.069</v>
+      </c>
+    </row>
+    <row r="32" hidden="1">
       <c r="A32" s="1">
         <v>21.0</v>
       </c>
@@ -1314,10 +1326,10 @@
         <v>2.0</v>
       </c>
       <c r="C32" s="1">
-        <v>3.717</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>2.837</v>
+      </c>
+    </row>
+    <row r="33" hidden="1">
       <c r="A33" s="1">
         <v>21.0</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>4.0</v>
       </c>
       <c r="C33" s="1">
-        <v>3.619</v>
+        <v>2.768</v>
       </c>
     </row>
     <row r="34">
@@ -1336,10 +1348,10 @@
         <v>6.0</v>
       </c>
       <c r="C34" s="1">
-        <v>2.993</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>3.074</v>
+      </c>
+    </row>
+    <row r="35" hidden="1">
       <c r="A35" s="1">
         <v>22.0</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>4.0</v>
       </c>
       <c r="C35" s="1">
-        <v>4.408</v>
+        <v>3.148</v>
       </c>
     </row>
     <row r="36">
@@ -1358,10 +1370,10 @@
         <v>6.0</v>
       </c>
       <c r="C36" s="1">
-        <v>2.918</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>2.758</v>
+      </c>
+    </row>
+    <row r="37" hidden="1">
       <c r="A37" s="1">
         <v>23.0</v>
       </c>
@@ -1369,7 +1381,7 @@
         <v>4.0</v>
       </c>
       <c r="C37" s="1">
-        <v>4.543</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="38">
@@ -1380,10 +1392,10 @@
         <v>6.0</v>
       </c>
       <c r="C38" s="1">
-        <v>2.871</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>2.73</v>
+      </c>
+    </row>
+    <row r="39" hidden="1">
       <c r="A39" s="1">
         <v>24.0</v>
       </c>
@@ -1391,7 +1403,7 @@
         <v>4.0</v>
       </c>
       <c r="C39" s="1">
-        <v>4.545</v>
+        <v>3.14</v>
       </c>
     </row>
     <row r="40">
@@ -1402,11 +1414,17 @@
         <v>6.0</v>
       </c>
       <c r="C40" s="1">
-        <v>2.659</v>
+        <v>3.045</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$C$40"/>
+  <autoFilter ref="$A$1:$C$40">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1440,7 +1458,7 @@
         <v>2.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1.603</v>
+        <v>1.834</v>
       </c>
     </row>
     <row r="3">
@@ -1451,7 +1469,7 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1">
-        <v>1.645</v>
+        <v>1.531</v>
       </c>
     </row>
     <row r="4">
@@ -1462,7 +1480,7 @@
         <v>2.0</v>
       </c>
       <c r="C4" s="1">
-        <v>1.839</v>
+        <v>1.51</v>
       </c>
     </row>
     <row r="5">
@@ -1473,7 +1491,7 @@
         <v>2.0</v>
       </c>
       <c r="C5" s="1">
-        <v>1.89</v>
+        <v>1.533</v>
       </c>
     </row>
     <row r="6">
@@ -1484,7 +1502,7 @@
         <v>2.0</v>
       </c>
       <c r="C6" s="1">
-        <v>1.874</v>
+        <v>1.539</v>
       </c>
     </row>
     <row r="7">
@@ -1495,7 +1513,7 @@
         <v>2.0</v>
       </c>
       <c r="C7" s="1">
-        <v>1.895</v>
+        <v>1.53</v>
       </c>
     </row>
     <row r="8">
@@ -1506,7 +1524,7 @@
         <v>2.0</v>
       </c>
       <c r="C8" s="1">
-        <v>1.906</v>
+        <v>1.654</v>
       </c>
     </row>
     <row r="9">
@@ -1517,7 +1535,7 @@
         <v>2.0</v>
       </c>
       <c r="C9" s="1">
-        <v>1.853</v>
+        <v>1.552</v>
       </c>
     </row>
     <row r="10">
@@ -1528,7 +1546,7 @@
         <v>2.0</v>
       </c>
       <c r="C10" s="1">
-        <v>1.869</v>
+        <v>1.582</v>
       </c>
     </row>
     <row r="11">
@@ -1539,7 +1557,7 @@
         <v>2.0</v>
       </c>
       <c r="C11" s="1">
-        <v>1.864</v>
+        <v>1.507</v>
       </c>
     </row>
     <row r="12">
@@ -1550,7 +1568,7 @@
         <v>2.0</v>
       </c>
       <c r="C12" s="1">
-        <v>1.895</v>
+        <v>1.521</v>
       </c>
     </row>
     <row r="13">
@@ -1561,7 +1579,7 @@
         <v>2.0</v>
       </c>
       <c r="C13" s="1">
-        <v>3.74</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="14">
@@ -1572,7 +1590,7 @@
         <v>2.0</v>
       </c>
       <c r="C14" s="1">
-        <v>3.647</v>
+        <v>2.968</v>
       </c>
     </row>
     <row r="15">
@@ -1583,7 +1601,7 @@
         <v>2.0</v>
       </c>
       <c r="C15" s="1">
-        <v>3.717</v>
+        <v>2.837</v>
       </c>
     </row>
   </sheetData>
@@ -1620,7 +1638,7 @@
         <v>4.0</v>
       </c>
       <c r="C2" s="1">
-        <v>1.756</v>
+        <v>1.746</v>
       </c>
     </row>
     <row r="3">
@@ -1631,7 +1649,7 @@
         <v>4.0</v>
       </c>
       <c r="C3" s="1">
-        <v>3.324</v>
+        <v>1.661</v>
       </c>
     </row>
     <row r="4">
@@ -1642,7 +1660,7 @@
         <v>4.0</v>
       </c>
       <c r="C4" s="1">
-        <v>3.283</v>
+        <v>1.696</v>
       </c>
     </row>
     <row r="5">
@@ -1653,7 +1671,7 @@
         <v>4.0</v>
       </c>
       <c r="C5" s="1">
-        <v>3.374</v>
+        <v>1.993</v>
       </c>
     </row>
     <row r="6">
@@ -1664,7 +1682,7 @@
         <v>4.0</v>
       </c>
       <c r="C6" s="1">
-        <v>3.392</v>
+        <v>1.893</v>
       </c>
     </row>
     <row r="7">
@@ -1675,7 +1693,7 @@
         <v>4.0</v>
       </c>
       <c r="C7" s="1">
-        <v>3.406</v>
+        <v>1.628</v>
       </c>
     </row>
     <row r="8">
@@ -1686,7 +1704,7 @@
         <v>4.0</v>
       </c>
       <c r="C8" s="1">
-        <v>3.385</v>
+        <v>2.025</v>
       </c>
     </row>
     <row r="9">
@@ -1697,7 +1715,7 @@
         <v>4.0</v>
       </c>
       <c r="C9" s="1">
-        <v>3.386</v>
+        <v>1.901</v>
       </c>
     </row>
     <row r="10">
@@ -1708,7 +1726,7 @@
         <v>4.0</v>
       </c>
       <c r="C10" s="1">
-        <v>3.409</v>
+        <v>1.771</v>
       </c>
     </row>
     <row r="11">
@@ -1719,7 +1737,7 @@
         <v>4.0</v>
       </c>
       <c r="C11" s="1">
-        <v>3.424</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="12">
@@ -1730,7 +1748,7 @@
         <v>4.0</v>
       </c>
       <c r="C12" s="1">
-        <v>3.665</v>
+        <v>2.734</v>
       </c>
     </row>
     <row r="13">
@@ -1741,7 +1759,7 @@
         <v>4.0</v>
       </c>
       <c r="C13" s="1">
-        <v>3.606</v>
+        <v>2.773</v>
       </c>
     </row>
     <row r="14">
@@ -1752,7 +1770,7 @@
         <v>4.0</v>
       </c>
       <c r="C14" s="1">
-        <v>3.619</v>
+        <v>2.768</v>
       </c>
     </row>
     <row r="15">
@@ -1763,7 +1781,7 @@
         <v>4.0</v>
       </c>
       <c r="C15" s="1">
-        <v>4.408</v>
+        <v>3.148</v>
       </c>
     </row>
     <row r="16">
@@ -1774,7 +1792,7 @@
         <v>4.0</v>
       </c>
       <c r="C16" s="1">
-        <v>4.543</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="17">
@@ -1785,7 +1803,7 @@
         <v>4.0</v>
       </c>
       <c r="C17" s="1">
-        <v>4.545</v>
+        <v>3.14</v>
       </c>
     </row>
   </sheetData>
@@ -1822,7 +1840,7 @@
         <v>6.0</v>
       </c>
       <c r="C2" s="1">
-        <v>2.163</v>
+        <v>2.028</v>
       </c>
     </row>
     <row r="3">
@@ -1833,7 +1851,7 @@
         <v>6.0</v>
       </c>
       <c r="C3" s="1">
-        <v>2.119</v>
+        <v>2.115</v>
       </c>
     </row>
     <row r="4">
@@ -1844,7 +1862,7 @@
         <v>6.0</v>
       </c>
       <c r="C4" s="1">
-        <v>2.195</v>
+        <v>2.287</v>
       </c>
     </row>
     <row r="5">
@@ -1855,7 +1873,7 @@
         <v>6.0</v>
       </c>
       <c r="C5" s="1">
-        <v>3.023</v>
+        <v>3.044</v>
       </c>
     </row>
     <row r="6">
@@ -1866,7 +1884,7 @@
         <v>6.0</v>
       </c>
       <c r="C6" s="1">
-        <v>3.068</v>
+        <v>3.069</v>
       </c>
     </row>
     <row r="7">
@@ -1877,7 +1895,7 @@
         <v>6.0</v>
       </c>
       <c r="C7" s="1">
-        <v>2.993</v>
+        <v>3.074</v>
       </c>
     </row>
     <row r="8">
@@ -1888,7 +1906,7 @@
         <v>6.0</v>
       </c>
       <c r="C8" s="1">
-        <v>2.918</v>
+        <v>2.758</v>
       </c>
     </row>
     <row r="9">
@@ -1899,7 +1917,7 @@
         <v>6.0</v>
       </c>
       <c r="C9" s="1">
-        <v>2.871</v>
+        <v>2.73</v>
       </c>
     </row>
     <row r="10">
@@ -1910,7 +1928,174 @@
         <v>6.0</v>
       </c>
       <c r="C10" s="1">
-        <v>2.659</v>
+        <v>3.045</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:B17" si="1">floor(log10(pow(2,8*A2-1) - 1),1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>